<commit_message>
updated files from tufts bceu, becf, bhrbef, bpcbs, bfpat, baadtbvt
</commit_message>
<xml_diff>
--- a/InputData/elec/BTC/BAU Transmission Capacity.xlsx
+++ b/InputData/elec/BTC/BAU Transmission Capacity.xlsx
@@ -376,7 +376,7 @@
     <xdr:ext cx="5219700" cy="2905125"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -404,7 +404,7 @@
     <xdr:ext cx="5219700" cy="1581150"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>

</xml_diff>